<commit_message>
EPBDS-12566 Adding test coverage for Numbers & decision tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Numbers.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aromashko/openl/src/openl-tablets/STUDIO/org.openl.rules.test/test-resources/functionality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpushko/EIS/1. EPBDS/EPBDS-12566/14 03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A22E0AF-00BD-FE49-9FC6-57E2166EDFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EB42A8-4834-D84D-B594-EF7A28895D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="1720" windowWidth="23900" windowHeight="13840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Env" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Float" sheetId="6" r:id="rId4"/>
     <sheet name="BigInteger" sheetId="3" r:id="rId5"/>
     <sheet name="BigDecimal" sheetId="4" r:id="rId6"/>
-    <sheet name="Byte, Short, Long" sheetId="5" r:id="rId7"/>
+    <sheet name="Byte, Short, Long, Char" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="138">
   <si>
     <t>Method String integerToString(Integer integer)</t>
   </si>
@@ -339,24 +339,15 @@
     <t>Test byteToString</t>
   </si>
   <si>
-    <t>Method String byteToString(byte number)</t>
-  </si>
-  <si>
     <t>return toString(number);</t>
   </si>
   <si>
     <t>number</t>
   </si>
   <si>
-    <t>Method String shortToString(short number)</t>
-  </si>
-  <si>
     <t>Test shortToString</t>
   </si>
   <si>
-    <t>Method String longToString(long number)</t>
-  </si>
-  <si>
     <t>Test longToString</t>
   </si>
   <si>
@@ -409,6 +400,51 @@
   </si>
   <si>
     <t>Doesn't pass because of EPBDS-8218. See org.openl.rules.convertor.String2BigDecimalConvertor</t>
+  </si>
+  <si>
+    <t>Method String byteToString(Byte number)</t>
+  </si>
+  <si>
+    <t>Method String shortToString(Short number)</t>
+  </si>
+  <si>
+    <t>Method String longToString(Long number)</t>
+  </si>
+  <si>
+    <t>_description_</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Verify null</t>
+  </si>
+  <si>
+    <t>Test charToString</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>∞</t>
+  </si>
+  <si>
+    <t>Method String charToString(Character number)</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -428,15 +464,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -444,18 +486,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,15 +901,15 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -798,10 +919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F28"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -815,262 +936,296 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5">
+      <c r="D5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D6" s="5"/>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D7" s="5"/>
+      <c r="E7" s="14">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5">
         <v>100</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F8" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5">
         <v>-100</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F9" s="6">
         <v>-100</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D7">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D18" s="5">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D19" s="5">
+        <v>100</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D20" s="5">
+        <v>100</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="5">
+        <v>100</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D22" s="5">
+        <v>100</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="5">
+        <v>10000</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D24" s="5">
+        <v>12000</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D26" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D30" s="5"/>
+      <c r="E30" s="6">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D13">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D14">
-        <v>100</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D15">
-        <v>100</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D16">
-        <v>100</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D17">
-        <v>100</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D18">
-        <v>10000</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D19">
-        <v>12000</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D20">
+      <c r="F30" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D21">
-        <v>-1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E25" s="4">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D26">
+      <c r="E31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E27" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>115</v>
+      <c r="E33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D15:F15"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -1082,307 +1237,346 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2FBBDD-B67E-E04B-8BC5-3FBCCBC170CF}">
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView zoomScale="128" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E11"/>
+    <sheetView topLeftCell="A16" zoomScale="128" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="55.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+      <c r="D4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13">
         <v>100.5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>119</v>
+      <c r="F6" s="18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D7" s="5">
+      <c r="D7" s="13"/>
+      <c r="E7" s="19">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D8" s="13"/>
+      <c r="E8" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D8" s="5">
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D9" s="13"/>
+      <c r="E9" s="20">
         <v>1000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F9" s="18">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D9" s="5">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D10" s="13"/>
+      <c r="E10" s="20">
         <v>-1000</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F10" s="18">
         <v>-1000</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D10" s="5">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D11" s="13"/>
+      <c r="E11" s="20">
         <v>0.01</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F11" s="18">
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D11" s="5">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D12" s="13"/>
+      <c r="E12" s="20">
         <v>-0.01</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F12" s="18">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D12" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="1" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D17" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D18" s="5">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D19" s="17">
         <v>100.5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D19" s="5">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D20" s="17">
         <v>100.5</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D20" s="5">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="17">
         <v>100.5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F21" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D21" s="5">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D22" s="17">
         <v>100.51</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D22" s="5">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="17">
         <v>10000.5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D23" s="5">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D24" s="17">
         <v>0.12</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D24" s="5">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D25" s="17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D25" s="5">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D26" s="17">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F26" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D26" s="5">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D27" s="17">
         <v>0.03</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F27" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D27" s="5">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D28" s="17">
         <v>0.03</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D28" s="5">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D29" s="17">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E29" s="4">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D30" s="5"/>
+      <c r="E30" s="6">
         <v>0</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D30">
+      <c r="F30" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D32">
+      <c r="E31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>115</v>
+      <c r="E33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D16:F16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1390,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801EB7DF-1CEA-CE47-B91E-276453D5AE28}">
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1401,259 +1595,291 @@
     <col min="2" max="2" width="56.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>93</v>
       </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
         <v>100.5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D6" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E13" t="s">
-        <v>115</v>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
+      <c r="D15" s="17">
+        <v>100.5</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
+      <c r="D16" s="17">
+        <v>100.5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
+      <c r="D17" s="17">
+        <v>100.5</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D18" s="5">
-        <v>100.5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
+      <c r="D18" s="17">
+        <v>100.51</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D19" s="5">
-        <v>100.5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
+      <c r="D19" s="17">
+        <v>10000.5</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D20" s="5">
-        <v>100.5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="4">
-        <v>100</v>
+      <c r="D20" s="17">
+        <v>0.12</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D21" s="5">
-        <v>100.51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>32</v>
+      <c r="D21" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D22" s="5">
-        <v>10000.5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>34</v>
+      <c r="D22" s="17">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D23" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>35</v>
+      <c r="D23" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D24" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>36</v>
+      <c r="D24" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D25" s="5">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>37</v>
+      <c r="D25" s="17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D26" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>53</v>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.15">
       <c r="D27" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="E27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D28" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
-        <v>39</v>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D30">
+      <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>115</v>
+      <c r="E29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB6630A-8DA6-FC41-B823-07B8C3651EDF}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="C1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1669,469 +1895,538 @@
       <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D6" s="5"/>
+      <c r="E6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B9" s="1" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D8" s="11"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D11" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D12" s="6" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D13" s="6" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D14" s="6" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D15" s="6" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F16" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D16" s="6" t="s">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D17" s="6" t="s">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D18" s="6" t="s">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E19" s="4">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D20" s="5"/>
+      <c r="E20" s="6">
         <v>0</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D20">
+      <c r="F20" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>115</v>
+      <c r="E21" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D22">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="5">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>115</v>
+      <c r="E23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D10:F10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744742AB-0F03-DF40-A4C9-7933578E7957}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="131" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="131" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="23" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5" s="6" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D5" s="5"/>
+      <c r="E5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D6" s="6" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D6" s="5"/>
+      <c r="E6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D7" s="4">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D8" s="4">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D9" s="4" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D11" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D13" s="4">
+      <c r="E13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="6">
         <v>1000</v>
       </c>
-      <c r="E13" s="4">
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="6">
         <v>1000</v>
       </c>
-      <c r="F13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D14" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="F14" s="6">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" s="23" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>82</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D19" s="6" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D20" s="6" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D21" s="6" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D22" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D22" s="6" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D23" s="6" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D24" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D24" s="6" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D25" s="6" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F26" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E26" s="4">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D27" s="5"/>
+      <c r="E27" s="6">
         <v>0</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D27">
+      <c r="F27" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>115</v>
+      <c r="E28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D29">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>115</v>
+      <c r="E30" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D17:F17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75753974-5D8B-B043-AB86-592F2B2FE267}">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:H40"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2140,161 +2435,377 @@
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6">
+        <v>100</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5">
+        <v>-120</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-120</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="1"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D4" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F12" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D6">
-        <v>-120</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B8" s="1" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <v>-1200</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="E17" s="4"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F20" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D10" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D11">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="4" t="s">
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D24" s="5"/>
+      <c r="E24" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D25" s="5"/>
+      <c r="E25" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D12">
-        <v>-1200</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
+      <c r="F25" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B28" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B29" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D16" t="s">
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D30" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D17" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="D18" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D28:F28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>